<commit_message>
Added ipython notebook 'Experiment2'
</commit_message>
<xml_diff>
--- a/src/Gabriel/ML_Workbook_1/Findings/Univariate Feature Ranking.xlsx
+++ b/src/Gabriel/ML_Workbook_1/Findings/Univariate Feature Ranking.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Lag0" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="372" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="400" uniqueCount="126">
   <si>
     <t>Mutual Information Rankings</t>
   </si>
@@ -311,13 +311,97 @@
   </si>
   <si>
     <t>var2(t-4)</t>
+  </si>
+  <si>
+    <t>var6(t-1)     0.062611</t>
+  </si>
+  <si>
+    <t>var6(t)       0.059204</t>
+  </si>
+  <si>
+    <t>var7(t)       0.051672</t>
+  </si>
+  <si>
+    <t>var7(t-1)     0.050866</t>
+  </si>
+  <si>
+    <t>var2(t)       0.049554</t>
+  </si>
+  <si>
+    <t>var2(t-1)     0.047698</t>
+  </si>
+  <si>
+    <t>var13(t-1)    0.045910</t>
+  </si>
+  <si>
+    <t>var13(t)      0.044309</t>
+  </si>
+  <si>
+    <t>var1(t)       0.040046</t>
+  </si>
+  <si>
+    <t>var1(t-1)     0.039134</t>
+  </si>
+  <si>
+    <t>var14(t-1)    0.039078</t>
+  </si>
+  <si>
+    <t>var4(t-1)     0.035342</t>
+  </si>
+  <si>
+    <t>var14(t)      0.035331</t>
+  </si>
+  <si>
+    <t>var4(t)       0.034682</t>
+  </si>
+  <si>
+    <t>var11(t-1)    0.032368</t>
+  </si>
+  <si>
+    <t>var11(t)      0.031154</t>
+  </si>
+  <si>
+    <t>var12(t)      0.029660</t>
+  </si>
+  <si>
+    <t>var3(t-1)     0.029289</t>
+  </si>
+  <si>
+    <t>var12(t-1)    0.028481</t>
+  </si>
+  <si>
+    <t>var3(t)       0.028352</t>
+  </si>
+  <si>
+    <t>var5(t-1)     0.025847</t>
+  </si>
+  <si>
+    <t>var5(t)       0.025732</t>
+  </si>
+  <si>
+    <t>var8(t-1)     0.025523</t>
+  </si>
+  <si>
+    <t>var10(t)      0.025306</t>
+  </si>
+  <si>
+    <t>var10(t-1)    0.024516</t>
+  </si>
+  <si>
+    <t>var8(t)       0.024122</t>
+  </si>
+  <si>
+    <t>var9(t)       0.017511</t>
+  </si>
+  <si>
+    <t>var9(t-1)     0.016705</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -332,6 +416,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Courier New"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="2">
@@ -354,11 +444,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -662,7 +755,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
@@ -1394,10 +1487,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F37"/>
+  <dimension ref="A1:H37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D44" sqref="D44"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1409,7 +1502,7 @@
     <col min="5" max="5" width="21" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>46</v>
       </c>
@@ -1419,283 +1512,315 @@
       <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>16</v>
-      </c>
       <c r="E1" s="1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H1" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>49</v>
       </c>
       <c r="C2">
         <v>5.2671950083934098E-2</v>
       </c>
-      <c r="D2">
-        <v>2.1273E-2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H2" s="4" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>50</v>
       </c>
       <c r="C3">
         <v>4.8359553870532E-2</v>
       </c>
-      <c r="D3">
-        <v>2.0209999999999999E-2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H3" s="4" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>8</v>
       </c>
       <c r="C4">
         <v>5.2902232101920403E-2</v>
       </c>
-      <c r="D4">
-        <v>2.0094999999999998E-2</v>
-      </c>
       <c r="E4">
         <v>1.704143</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H4" s="4" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>7</v>
       </c>
       <c r="C5">
         <v>4.8254542006968201E-2</v>
       </c>
-      <c r="D5">
-        <v>1.8957000000000002E-2</v>
-      </c>
       <c r="E5">
         <v>-0.374863</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H5" s="4" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>3</v>
       </c>
       <c r="C6">
         <v>2.4475902204953499E-2</v>
       </c>
-      <c r="D6">
-        <v>1.3859E-2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H6" s="4" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>47</v>
       </c>
       <c r="C7">
         <v>5.5273608041389297E-2</v>
       </c>
-      <c r="D7">
-        <v>1.2614999999999999E-2</v>
-      </c>
       <c r="E7">
         <v>3.7318470000000001</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H7" s="4" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>54</v>
       </c>
       <c r="C8">
         <v>2.43707181246119E-2</v>
       </c>
-      <c r="D8">
-        <v>1.2282E-2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H8" s="4" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>48</v>
       </c>
       <c r="C9">
         <v>5.3008007501495903E-2</v>
       </c>
-      <c r="D9">
-        <v>1.1953999999999999E-2</v>
-      </c>
       <c r="E9">
         <v>2.669073</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H9" s="4" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>2</v>
       </c>
       <c r="C10">
         <v>5.4505259203662997E-2</v>
       </c>
-      <c r="D10">
-        <v>1.0532E-2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H10" s="4" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>15</v>
       </c>
       <c r="C11">
         <v>5.2519932641015003E-2</v>
       </c>
-      <c r="D11">
-        <v>1.0129000000000001E-2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H11" s="4" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>51</v>
       </c>
       <c r="C12">
         <v>3.9597879072907398E-2</v>
       </c>
-      <c r="D12">
-        <v>9.4299999999999991E-3</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H12" s="4" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>14</v>
       </c>
       <c r="C13">
         <v>3.9554551708196002E-2</v>
       </c>
-      <c r="D13">
-        <v>9.3189999999999992E-3</v>
-      </c>
       <c r="E13">
         <v>2.3743750000000001</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H13" s="4" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>13</v>
       </c>
       <c r="C14">
         <v>2.9025760810825502E-2</v>
       </c>
-      <c r="D14">
-        <v>6.7499999999999999E-3</v>
-      </c>
       <c r="E14">
         <v>2.0562740000000002</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H14" s="4" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>52</v>
       </c>
       <c r="C15">
         <v>2.97188518116757E-2</v>
       </c>
-      <c r="D15">
-        <v>6.7359999999999998E-3</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H15" s="4" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>53</v>
       </c>
       <c r="C16">
         <v>2.8438686620760899E-2</v>
       </c>
-      <c r="D16">
-        <v>5.0299999999999997E-3</v>
-      </c>
       <c r="E16">
         <v>0.19115099999999999</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H16" s="4" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>12</v>
       </c>
       <c r="C17">
         <v>2.79000229719066E-2</v>
       </c>
-      <c r="D17">
-        <v>4.6569999999999997E-3</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H17" s="4" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>6</v>
       </c>
       <c r="E18">
         <v>9.024051</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H18" s="4" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>55</v>
       </c>
       <c r="E19">
         <v>2.7442859999999998</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H19" s="4" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>56</v>
       </c>
       <c r="E20">
         <v>1.6092550000000001</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H20" s="4" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>4</v>
       </c>
       <c r="E21">
         <v>1.153934</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H21" s="4" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>9</v>
       </c>
       <c r="E22">
         <v>0.80480300000000005</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H22" s="4" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
         <v>57</v>
       </c>
       <c r="E23">
         <v>0.75151199999999996</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H23" s="4" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
         <v>5</v>
       </c>
       <c r="E24">
         <v>-0.46449600000000002</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H24" s="4" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
         <v>58</v>
       </c>
       <c r="E25">
         <v>-0.78993100000000005</v>
       </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H25" s="4" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
         <v>10</v>
       </c>
       <c r="E26">
         <v>-1.1063480000000001</v>
       </c>
-    </row>
-    <row r="28" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H26" s="4" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H27" s="4" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>19</v>
       </c>
@@ -1714,8 +1839,11 @@
       <c r="F28" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H28" s="4" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>23</v>
       </c>
@@ -1734,8 +1862,11 @@
       <c r="F29" s="2">
         <v>0.44426412295000001</v>
       </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H29" s="4" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>23</v>
       </c>
@@ -1755,7 +1886,7 @@
         <v>0.52607857823500004</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>23</v>
       </c>
@@ -1775,7 +1906,7 @@
         <v>0.45425766850900001</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>23</v>
       </c>

</xml_diff>